<commit_message>
Added Analysis for Alphaopic and Age-dependent measures. Also changed how the analysis modules interact with the central information branch
</commit_message>
<xml_diff>
--- a/data-raw/languages.xlsx
+++ b/data-raw/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Gremienarbeit/TWA/Projekte/Spectran/Spectran/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269CD900-4221-6444-A56D-48261C62C275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5134B977-4708-6849-8F92-DB0B4B404ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20460" yWindow="5180" windowWidth="29080" windowHeight="18880" activeTab="2" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
+    <workbookView xWindow="17180" yWindow="3400" windowWidth="29080" windowHeight="18880" activeTab="2" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="1" r:id="rId1"/>
@@ -1384,15 +1384,9 @@
     <t>Integral of the spectral irradiance</t>
   </si>
   <si>
-    <t>Wellenlänge mit der höchsten Bestrahlungsstärke</t>
-  </si>
-  <si>
     <t>Bewertet wird nur der visuelle Bereich, d.h. Wellenlängen zwischen 380 und 780 nm.</t>
   </si>
   <si>
-    <t>Wavelength with the highest spectral value</t>
-  </si>
-  <si>
     <t>Integral der spektralen Photonenflussdichte</t>
   </si>
   <si>
@@ -1585,9 +1579,6 @@
     <t>Correction factor for the transmission of ocular media</t>
   </si>
   <si>
-    <t>age-related correction factor for melanopic light effects</t>
-  </si>
-  <si>
     <t xml:space="preserve">MEDI for a </t>
   </si>
   <si>
@@ -1894,9 +1885,6 @@
     <t>Cyanopic evaluation (short wavelength cone)</t>
   </si>
   <si>
-    <t>Rhodopic evaluation (skotopic vision)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> aber verwenden? Schicken Sie dem </t>
   </si>
   <si>
@@ -1964,6 +1952,18 @@
   </si>
   <si>
     <t>CIE Standard Illuminant</t>
+  </si>
+  <si>
+    <t>Rhodopic evaluation (scotopic vision)</t>
+  </si>
+  <si>
+    <t>Wavelength with the highest spectral value (or the mean, if there are several)</t>
+  </si>
+  <si>
+    <t>Wellenlänge mit der höchsten Bestrahlungsstärke (oder deren Mittelwert, wenn es mehrere gibt)</t>
+  </si>
+  <si>
+    <t>Age-related correction factor for melanopic light effects</t>
   </si>
 </sst>
 </file>
@@ -2331,7 +2331,7 @@
   <dimension ref="A1:E168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2465,7 +2465,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2483,7 +2483,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2501,7 +2501,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2519,7 +2519,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2537,7 +2537,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2555,7 +2555,7 @@
         <v>146</v>
       </c>
       <c r="E12" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3035,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16C6AC7-F954-EC4A-BACE-CEC04494FD73}">
   <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3185,7 +3185,7 @@
         <v>lang$ui(7)</v>
       </c>
       <c r="D8" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
@@ -3548,7 +3548,7 @@
         <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3926,7 +3926,7 @@
         <v>116</v>
       </c>
       <c r="E49" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -4211,10 +4211,10 @@
         <v>lang$ui(64)</v>
       </c>
       <c r="D65" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="E65" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4283,10 +4283,10 @@
         <v>lang$ui(68)</v>
       </c>
       <c r="D69" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="E69" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4805,7 +4805,7 @@
         <v>lang$ui(97)</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>214</v>
@@ -4967,7 +4967,7 @@
         <v>lang$ui(106)</v>
       </c>
       <c r="D107" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E107" t="s">
         <v>250</v>
@@ -6083,10 +6083,10 @@
         <v>lang$ui(168)</v>
       </c>
       <c r="D169" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="E169" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -6101,10 +6101,10 @@
         <v>lang$ui(169)</v>
       </c>
       <c r="D170" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E170" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -6119,10 +6119,10 @@
         <v>lang$ui(170)</v>
       </c>
       <c r="D171" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="E171" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -6134,8 +6134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496328DD-5C8E-3D45-AB81-313F176488D7}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6966,10 +6966,10 @@
         <v>lang$server(45)</v>
       </c>
       <c r="D46" t="s">
-        <v>448</v>
+        <v>640</v>
       </c>
       <c r="E46" t="s">
-        <v>450</v>
+        <v>639</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -6984,10 +6984,10 @@
         <v>lang$server(46)</v>
       </c>
       <c r="D47" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E47" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -7002,10 +7002,10 @@
         <v>lang$server(47)</v>
       </c>
       <c r="D48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E48" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -7020,10 +7020,10 @@
         <v>lang$server(48)</v>
       </c>
       <c r="D49" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E49" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -7038,10 +7038,10 @@
         <v>lang$server(49)</v>
       </c>
       <c r="D50" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E50" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -7056,10 +7056,10 @@
         <v>lang$server(50)</v>
       </c>
       <c r="D51" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E51" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -7074,10 +7074,10 @@
         <v>lang$server(51)</v>
       </c>
       <c r="D52" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E52" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -7092,10 +7092,10 @@
         <v>lang$server(52)</v>
       </c>
       <c r="D53" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E53" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -7110,10 +7110,10 @@
         <v>lang$server(53)</v>
       </c>
       <c r="D54" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E54" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -7146,10 +7146,10 @@
         <v>lang$server(55)</v>
       </c>
       <c r="D56" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E56" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -7164,10 +7164,10 @@
         <v>lang$server(56)</v>
       </c>
       <c r="D57" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E57" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -7182,7 +7182,7 @@
         <v>lang$server(57)</v>
       </c>
       <c r="D58" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E58" t="s">
         <v>159</v>
@@ -7200,10 +7200,10 @@
         <v>lang$server(58)</v>
       </c>
       <c r="D59" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E59" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -7218,10 +7218,10 @@
         <v>lang$server(59)</v>
       </c>
       <c r="D60" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E60" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -7236,10 +7236,10 @@
         <v>lang$server(60)</v>
       </c>
       <c r="D61" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E61" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -7254,10 +7254,10 @@
         <v>lang$server(61)</v>
       </c>
       <c r="D62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E62" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -7272,10 +7272,10 @@
         <v>lang$server(62)</v>
       </c>
       <c r="D63" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E63" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -7293,7 +7293,7 @@
         <v>201</v>
       </c>
       <c r="E64" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -7308,10 +7308,10 @@
         <v>lang$server(64)</v>
       </c>
       <c r="D65" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E65" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -7326,10 +7326,10 @@
         <v>lang$server(65)</v>
       </c>
       <c r="D66" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E66" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -7344,10 +7344,10 @@
         <v>lang$server(66)</v>
       </c>
       <c r="D67" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E67" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -7362,10 +7362,10 @@
         <v>lang$server(67)</v>
       </c>
       <c r="D68" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E68" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -7380,10 +7380,10 @@
         <v>lang$server(68)</v>
       </c>
       <c r="D69" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E69" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -7398,10 +7398,10 @@
         <v>lang$server(69)</v>
       </c>
       <c r="D70" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E70" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -7416,10 +7416,10 @@
         <v>lang$server(70)</v>
       </c>
       <c r="D71" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E71" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -7434,10 +7434,10 @@
         <v>lang$server(71)</v>
       </c>
       <c r="D72" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E72" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -7452,10 +7452,10 @@
         <v>lang$server(72)</v>
       </c>
       <c r="D73" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E73" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -7470,15 +7470,15 @@
         <v>lang$server(73)</v>
       </c>
       <c r="D74" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E74" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -7488,15 +7488,15 @@
         <v>lang$server(74)</v>
       </c>
       <c r="D75" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E75" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -7506,15 +7506,15 @@
         <v>lang$server(75)</v>
       </c>
       <c r="D76" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E76" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -7524,15 +7524,15 @@
         <v>lang$server(76)</v>
       </c>
       <c r="D77" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E77" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -7542,15 +7542,15 @@
         <v>lang$server(77)</v>
       </c>
       <c r="D78" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E78" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -7560,15 +7560,15 @@
         <v>lang$server(78)</v>
       </c>
       <c r="D79" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E79" t="s">
-        <v>515</v>
+        <v>641</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -7578,15 +7578,15 @@
         <v>lang$server(79)</v>
       </c>
       <c r="D80" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E80" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -7596,15 +7596,15 @@
         <v>lang$server(80)</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B82">
         <v>81</v>
@@ -7614,15 +7614,15 @@
         <v>lang$server(81)</v>
       </c>
       <c r="D82" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E82" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B83">
         <v>82</v>
@@ -7632,15 +7632,15 @@
         <v>lang$server(82)</v>
       </c>
       <c r="D83" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E83" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -7650,15 +7650,15 @@
         <v>lang$server(83)</v>
       </c>
       <c r="D84" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E84" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -7668,15 +7668,15 @@
         <v>lang$server(84)</v>
       </c>
       <c r="D85" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E85" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -7686,15 +7686,15 @@
         <v>lang$server(85)</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -7704,15 +7704,15 @@
         <v>lang$server(86)</v>
       </c>
       <c r="D87" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B88">
         <v>87</v>
@@ -7722,15 +7722,15 @@
         <v>lang$server(87)</v>
       </c>
       <c r="D88" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E88" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B89">
         <v>88</v>
@@ -7740,15 +7740,15 @@
         <v>lang$server(88)</v>
       </c>
       <c r="D89" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E89" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -7758,15 +7758,15 @@
         <v>lang$server(89)</v>
       </c>
       <c r="D90" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E90" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B91">
         <v>90</v>
@@ -7776,15 +7776,15 @@
         <v>lang$server(90)</v>
       </c>
       <c r="D91" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E91" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -7794,15 +7794,15 @@
         <v>lang$server(91)</v>
       </c>
       <c r="D92" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E92" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B93">
         <v>92</v>
@@ -7812,15 +7812,15 @@
         <v>lang$server(92)</v>
       </c>
       <c r="D93" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E93" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B94">
         <v>93</v>
@@ -7830,15 +7830,15 @@
         <v>lang$server(93)</v>
       </c>
       <c r="D94" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E94" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B95">
         <v>94</v>
@@ -7848,15 +7848,15 @@
         <v>lang$server(94)</v>
       </c>
       <c r="D95" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B96">
         <v>95</v>
@@ -7866,15 +7866,15 @@
         <v>lang$server(95)</v>
       </c>
       <c r="D96" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E96" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B97">
         <v>96</v>
@@ -7884,15 +7884,15 @@
         <v>lang$server(96)</v>
       </c>
       <c r="D97" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B98">
         <v>97</v>
@@ -7902,15 +7902,15 @@
         <v>lang$server(97)</v>
       </c>
       <c r="D98" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E98" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B99">
         <v>98</v>
@@ -7920,15 +7920,15 @@
         <v>lang$server(98)</v>
       </c>
       <c r="D99" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E99" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -7938,15 +7938,15 @@
         <v>lang$server(99)</v>
       </c>
       <c r="D100" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E100" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B101">
         <v>100</v>
@@ -7956,7 +7956,7 @@
         <v>lang$server(100)</v>
       </c>
       <c r="D101" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E101" t="s">
         <v>422</v>
@@ -7964,7 +7964,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B102">
         <v>101</v>
@@ -7974,10 +7974,10 @@
         <v>lang$server(101)</v>
       </c>
       <c r="D102" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E102" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -7992,10 +7992,10 @@
         <v>lang$server(102)</v>
       </c>
       <c r="D103" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E103" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -8010,10 +8010,10 @@
         <v>lang$server(103)</v>
       </c>
       <c r="D104" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E104" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -8028,10 +8028,10 @@
         <v>lang$server(104)</v>
       </c>
       <c r="D105" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E105" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -8046,7 +8046,7 @@
         <v>lang$server(105)</v>
       </c>
       <c r="D106" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E106" t="s">
         <v>293</v>
@@ -8064,10 +8064,10 @@
         <v>lang$server(106)</v>
       </c>
       <c r="D107" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E107" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -8082,10 +8082,10 @@
         <v>lang$server(107)</v>
       </c>
       <c r="D108" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E108" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -8100,10 +8100,10 @@
         <v>lang$server(108)</v>
       </c>
       <c r="D109" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E109" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -8118,10 +8118,10 @@
         <v>lang$server(109)</v>
       </c>
       <c r="D110" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E110" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -8136,10 +8136,10 @@
         <v>lang$server(110)</v>
       </c>
       <c r="D111" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E111" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -8154,10 +8154,10 @@
         <v>lang$server(111)</v>
       </c>
       <c r="D112" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E112" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -8172,10 +8172,10 @@
         <v>lang$server(112)</v>
       </c>
       <c r="D113" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E113" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -8190,10 +8190,10 @@
         <v>lang$server(113)</v>
       </c>
       <c r="D114" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E114" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -8208,10 +8208,10 @@
         <v>lang$server(114)</v>
       </c>
       <c r="D115" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E115" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -8226,10 +8226,10 @@
         <v>lang$server(115)</v>
       </c>
       <c r="D116" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E116" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -8244,10 +8244,10 @@
         <v>lang$server(116)</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E117" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -8262,10 +8262,10 @@
         <v>lang$server(117)</v>
       </c>
       <c r="D118" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E118" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -8280,10 +8280,10 @@
         <v>lang$server(118)</v>
       </c>
       <c r="D119" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E119" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -8298,10 +8298,10 @@
         <v>lang$server(119)</v>
       </c>
       <c r="D120" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E120" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -8316,10 +8316,10 @@
         <v>lang$server(120)</v>
       </c>
       <c r="D121" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E121" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -8334,10 +8334,10 @@
         <v>lang$server(121)</v>
       </c>
       <c r="D122" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E122" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -8352,10 +8352,10 @@
         <v>lang$server(122)</v>
       </c>
       <c r="D123" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E123" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -8370,10 +8370,10 @@
         <v>lang$server(123)</v>
       </c>
       <c r="D124" t="s">
+        <v>594</v>
+      </c>
+      <c r="E124" t="s">
         <v>597</v>
-      </c>
-      <c r="E124" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -8388,10 +8388,10 @@
         <v>lang$server(124)</v>
       </c>
       <c r="D125" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E125" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -8406,10 +8406,10 @@
         <v>lang$server(125)</v>
       </c>
       <c r="D126" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E126" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -8424,10 +8424,10 @@
         <v>lang$server(126)</v>
       </c>
       <c r="D127" t="s">
+        <v>603</v>
+      </c>
+      <c r="E127" t="s">
         <v>606</v>
-      </c>
-      <c r="E127" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -8442,10 +8442,10 @@
         <v>lang$server(127)</v>
       </c>
       <c r="D128" t="s">
+        <v>604</v>
+      </c>
+      <c r="E128" t="s">
         <v>607</v>
-      </c>
-      <c r="E128" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -8460,10 +8460,10 @@
         <v>lang$server(128)</v>
       </c>
       <c r="D129" t="s">
+        <v>605</v>
+      </c>
+      <c r="E129" t="s">
         <v>608</v>
-      </c>
-      <c r="E129" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -8478,10 +8478,10 @@
         <v>lang$server(129)</v>
       </c>
       <c r="D130" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E130" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -8496,10 +8496,10 @@
         <v>lang$server(130)</v>
       </c>
       <c r="D131" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E131" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -8514,10 +8514,10 @@
         <v>lang$server(131)</v>
       </c>
       <c r="D132" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E132" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -8532,10 +8532,10 @@
         <v>lang$server(132)</v>
       </c>
       <c r="D133" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E133" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -8550,10 +8550,10 @@
         <v>lang$server(133)</v>
       </c>
       <c r="D134" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E134" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -8568,10 +8568,10 @@
         <v>lang$server(134)</v>
       </c>
       <c r="D135" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="E135" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finishing Work on Version 0.9.0.0
</commit_message>
<xml_diff>
--- a/data-raw/languages.xlsx
+++ b/data-raw/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Gremienarbeit/TWA/Projekte/Spectran/Spectran/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FF8353-E821-D946-BEE6-3E02D45CCE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A035851-D9C6-3846-AAB6-44623326C748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14440" yWindow="5460" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
+    <workbookView xWindow="15240" yWindow="5580" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="1" r:id="rId1"/>
@@ -1723,12 +1723,6 @@
     <t xml:space="preserve"> files were created.</t>
   </si>
   <si>
-    <t>Der Export wird vorbereitet. Die Dateien benötigen etwas Zeit zur Vorbereitung und stehen dann als Zip-Datei zum Herunterladen bereit.</t>
-  </si>
-  <si>
-    <t>Export files are prepared. They need a few moments to be ready for download as a ZIP-file.</t>
-  </si>
-  <si>
     <t>Die Dateien werden für den Download vorbereitet. Bitte haben Sie einen Moment Geduld.</t>
   </si>
   <si>
@@ -2003,6 +1997,12 @@
   </si>
   <si>
     <t>adjusted</t>
+  </si>
+  <si>
+    <t>Der Export wurde erfolgreich abgeschlossen.</t>
+  </si>
+  <si>
+    <t>Export was successful.</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2504,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2522,7 +2522,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2540,7 +2540,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2558,7 +2558,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2576,7 +2576,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2594,7 +2594,7 @@
         <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3074,8 +3074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16C6AC7-F954-EC4A-BACE-CEC04494FD73}">
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="D183" sqref="D183"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E149" sqref="E149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3224,7 +3224,7 @@
         <v>lang$ui(7)</v>
       </c>
       <c r="D8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
@@ -3692,10 +3692,10 @@
         <v>lang$ui(33)</v>
       </c>
       <c r="D34" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E34" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -4250,10 +4250,10 @@
         <v>lang$ui(64)</v>
       </c>
       <c r="D65" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E65" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4322,10 +4322,10 @@
         <v>lang$ui(68)</v>
       </c>
       <c r="D69" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E69" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4844,7 +4844,7 @@
         <v>lang$ui(97)</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>212</v>
@@ -5960,10 +5960,10 @@
         <v>lang$ui(159)</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E160" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -5978,10 +5978,10 @@
         <v>lang$ui(160)</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E161" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -5996,10 +5996,10 @@
         <v>lang$ui(161)</v>
       </c>
       <c r="D162" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E162" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -6014,10 +6014,10 @@
         <v>lang$ui(162)</v>
       </c>
       <c r="D163" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E163" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -6032,10 +6032,10 @@
         <v>lang$ui(163)</v>
       </c>
       <c r="D164" t="s">
+        <v>636</v>
+      </c>
+      <c r="E164" t="s">
         <v>638</v>
-      </c>
-      <c r="E164" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -6050,10 +6050,10 @@
         <v>lang$ui(164)</v>
       </c>
       <c r="D165" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E165" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -6068,10 +6068,10 @@
         <v>lang$ui(165)</v>
       </c>
       <c r="D166" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E166" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -6122,10 +6122,10 @@
         <v>lang$ui(168)</v>
       </c>
       <c r="D169" t="s">
+        <v>596</v>
+      </c>
+      <c r="E169" t="s">
         <v>598</v>
-      </c>
-      <c r="E169" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -6140,10 +6140,10 @@
         <v>lang$ui(169)</v>
       </c>
       <c r="D170" t="s">
+        <v>597</v>
+      </c>
+      <c r="E170" t="s">
         <v>599</v>
-      </c>
-      <c r="E170" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -6158,10 +6158,10 @@
         <v>lang$ui(170)</v>
       </c>
       <c r="D171" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E171" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -6176,10 +6176,10 @@
         <v>lang$ui(171)</v>
       </c>
       <c r="D172" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E172" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -6194,10 +6194,10 @@
         <v>lang$ui(172)</v>
       </c>
       <c r="D173" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E173" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -6212,10 +6212,10 @@
         <v>lang$ui(173)</v>
       </c>
       <c r="D174" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E174" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -6230,10 +6230,10 @@
         <v>lang$ui(174)</v>
       </c>
       <c r="D175" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E175" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -6248,10 +6248,10 @@
         <v>lang$ui(175)</v>
       </c>
       <c r="D176" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E176" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -6266,10 +6266,10 @@
         <v>lang$ui(176)</v>
       </c>
       <c r="D177" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E177" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -6284,10 +6284,10 @@
         <v>lang$ui(177)</v>
       </c>
       <c r="D178" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E178" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -6299,8 +6299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496328DD-5C8E-3D45-AB81-313F176488D7}">
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D141" sqref="D141"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7131,10 +7131,10 @@
         <v>lang$server(45)</v>
       </c>
       <c r="D46" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E46" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -7728,7 +7728,7 @@
         <v>490</v>
       </c>
       <c r="E79" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -7887,10 +7887,10 @@
         <v>lang$server(87)</v>
       </c>
       <c r="D88" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E88" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -8373,10 +8373,10 @@
         <v>lang$server(114)</v>
       </c>
       <c r="D115" t="s">
-        <v>561</v>
+        <v>653</v>
       </c>
       <c r="E115" t="s">
-        <v>562</v>
+        <v>654</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -8391,10 +8391,10 @@
         <v>lang$server(115)</v>
       </c>
       <c r="D116" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E116" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -8409,10 +8409,10 @@
         <v>lang$server(116)</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E117" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -8427,10 +8427,10 @@
         <v>lang$server(117)</v>
       </c>
       <c r="D118" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E118" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -8445,10 +8445,10 @@
         <v>lang$server(118)</v>
       </c>
       <c r="D119" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E119" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -8463,10 +8463,10 @@
         <v>lang$server(119)</v>
       </c>
       <c r="D120" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E120" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -8481,10 +8481,10 @@
         <v>lang$server(120)</v>
       </c>
       <c r="D121" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E121" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -8499,10 +8499,10 @@
         <v>lang$server(121)</v>
       </c>
       <c r="D122" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E122" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -8517,10 +8517,10 @@
         <v>lang$server(122)</v>
       </c>
       <c r="D123" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E123" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -8535,10 +8535,10 @@
         <v>lang$server(123)</v>
       </c>
       <c r="D124" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E124" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -8553,10 +8553,10 @@
         <v>lang$server(124)</v>
       </c>
       <c r="D125" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E125" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -8571,10 +8571,10 @@
         <v>lang$server(125)</v>
       </c>
       <c r="D126" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E126" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -8589,10 +8589,10 @@
         <v>lang$server(126)</v>
       </c>
       <c r="D127" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E127" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -8607,10 +8607,10 @@
         <v>lang$server(127)</v>
       </c>
       <c r="D128" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E128" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -8625,10 +8625,10 @@
         <v>lang$server(128)</v>
       </c>
       <c r="D129" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E129" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -8643,10 +8643,10 @@
         <v>lang$server(129)</v>
       </c>
       <c r="D130" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E130" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -8661,10 +8661,10 @@
         <v>lang$server(130)</v>
       </c>
       <c r="D131" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E131" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -8679,10 +8679,10 @@
         <v>lang$server(131)</v>
       </c>
       <c r="D132" t="s">
+        <v>603</v>
+      </c>
+      <c r="E132" t="s">
         <v>605</v>
-      </c>
-      <c r="E132" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -8697,10 +8697,10 @@
         <v>lang$server(132)</v>
       </c>
       <c r="D133" t="s">
+        <v>604</v>
+      </c>
+      <c r="E133" t="s">
         <v>606</v>
-      </c>
-      <c r="E133" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -8715,10 +8715,10 @@
         <v>lang$server(133)</v>
       </c>
       <c r="D134" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E134" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -8733,10 +8733,10 @@
         <v>lang$server(134)</v>
       </c>
       <c r="D135" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E135" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -8751,10 +8751,10 @@
         <v>lang$server(135)</v>
       </c>
       <c r="D136" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E136" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a conditional language changer (conditional on whether it is deployed on the shinyapps.io platform)
</commit_message>
<xml_diff>
--- a/data-raw/languages.xlsx
+++ b/data-raw/languages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Gremienarbeit/TWA/Projekte/Spectran/Spectran/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A035851-D9C6-3846-AAB6-44623326C748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039E9377-188E-9E4F-905F-E812145FAD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="5580" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
+    <workbookView xWindow="11680" yWindow="3040" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="662">
   <si>
     <t>Deutsch</t>
   </si>
@@ -994,9 +994,6 @@
     <t xml:space="preserve">Here, you can download graphs and tables from the </t>
   </si>
   <si>
-    <t xml:space="preserve"> section. Display options from that tab are kept for the export. For a few exceptions, export options can be overriden in the </t>
-  </si>
-  <si>
     <t>Validität</t>
   </si>
   <si>
@@ -2003,6 +2000,30 @@
   </si>
   <si>
     <t>Export was successful.</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>https://litg.shinyapps.io/Spectran_de/</t>
+  </si>
+  <si>
+    <t>https://litg.shinyapps.io/Spectran_en/</t>
+  </si>
+  <si>
+    <t>Zur Englischen Sprachversion</t>
+  </si>
+  <si>
+    <t>To the German version</t>
+  </si>
+  <si>
+    <t>earth-americas</t>
+  </si>
+  <si>
+    <t>earth-europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> section. Display options from that tab are kept for the export. For a few exceptions, export options can be overritten in the </t>
   </si>
 </sst>
 </file>
@@ -2367,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D99FFC6-0F2D-9847-9357-C8569C6C6BF8}">
-  <dimension ref="A1:E168"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2387,10 +2408,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2504,7 +2525,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2522,7 +2543,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2540,7 +2561,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2558,7 +2579,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2576,7 +2597,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2594,17 +2615,62 @@
         <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C13" s="3"/>
+      <c r="A13" t="s">
+        <v>654</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f t="shared" ref="C13:C15" si="1">"lang$global(" &amp; B13 &amp; ")"</f>
+        <v>lang$global(12)</v>
+      </c>
+      <c r="D13" t="s">
+        <v>657</v>
+      </c>
+      <c r="E13" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C14" s="3"/>
+      <c r="A14" t="s">
+        <v>654</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>lang$global(13)</v>
+      </c>
+      <c r="D14" t="s">
+        <v>659</v>
+      </c>
+      <c r="E14" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C15" s="3"/>
+      <c r="A15" t="s">
+        <v>654</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>lang$global(14)</v>
+      </c>
+      <c r="D15" t="s">
+        <v>656</v>
+      </c>
+      <c r="E15" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="3"/>
@@ -3064,6 +3130,9 @@
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C168" s="3"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C169" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3074,8 +3143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16C6AC7-F954-EC4A-BACE-CEC04494FD73}">
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E149" sqref="E149"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3092,10 +3161,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3224,7 +3293,7 @@
         <v>lang$ui(7)</v>
       </c>
       <c r="D8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
@@ -3587,7 +3656,7 @@
         <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3692,10 +3761,10 @@
         <v>lang$ui(33)</v>
       </c>
       <c r="D34" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E34" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -3965,7 +4034,7 @@
         <v>114</v>
       </c>
       <c r="E49" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -3980,10 +4049,10 @@
         <v>lang$ui(49)</v>
       </c>
       <c r="D50" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E50" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -3998,10 +4067,10 @@
         <v>lang$ui(50)</v>
       </c>
       <c r="D51" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E51" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -4250,10 +4319,10 @@
         <v>lang$ui(64)</v>
       </c>
       <c r="D65" t="s">
+        <v>611</v>
+      </c>
+      <c r="E65" t="s">
         <v>612</v>
-      </c>
-      <c r="E65" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4304,10 +4373,10 @@
         <v>lang$ui(67)</v>
       </c>
       <c r="D68" t="s">
+        <v>369</v>
+      </c>
+      <c r="E68" t="s">
         <v>370</v>
-      </c>
-      <c r="E68" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -4322,10 +4391,10 @@
         <v>lang$ui(68)</v>
       </c>
       <c r="D69" t="s">
+        <v>606</v>
+      </c>
+      <c r="E69" t="s">
         <v>607</v>
-      </c>
-      <c r="E69" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4628,10 +4697,10 @@
         <v>lang$ui(85)</v>
       </c>
       <c r="D86" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E86" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -4646,10 +4715,10 @@
         <v>lang$ui(86)</v>
       </c>
       <c r="D87" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E87" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -4844,7 +4913,7 @@
         <v>lang$ui(97)</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>212</v>
@@ -5006,7 +5075,7 @@
         <v>lang$ui(106)</v>
       </c>
       <c r="D107" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E107" t="s">
         <v>248</v>
@@ -5369,7 +5438,7 @@
         <v>263</v>
       </c>
       <c r="E127" t="s">
-        <v>318</v>
+        <v>661</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -5842,7 +5911,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B154">
         <v>153</v>
@@ -5852,15 +5921,15 @@
         <v>lang$ui(153)</v>
       </c>
       <c r="D154" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E154" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B155">
         <v>154</v>
@@ -5870,15 +5939,15 @@
         <v>lang$ui(154)</v>
       </c>
       <c r="D155" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E155" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B156">
         <v>155</v>
@@ -5888,15 +5957,15 @@
         <v>lang$ui(155)</v>
       </c>
       <c r="D156" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E156" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B157">
         <v>156</v>
@@ -5906,15 +5975,15 @@
         <v>lang$ui(156)</v>
       </c>
       <c r="D157" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E157" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B158">
         <v>157</v>
@@ -5924,15 +5993,15 @@
         <v>lang$ui(157)</v>
       </c>
       <c r="D158" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E158" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B159">
         <v>158</v>
@@ -5942,15 +6011,15 @@
         <v>lang$ui(158)</v>
       </c>
       <c r="D159" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E159" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B160">
         <v>159</v>
@@ -5960,15 +6029,15 @@
         <v>lang$ui(159)</v>
       </c>
       <c r="D160" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="E160" t="s">
         <v>634</v>
-      </c>
-      <c r="E160" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B161">
         <v>160</v>
@@ -5978,15 +6047,15 @@
         <v>lang$ui(160)</v>
       </c>
       <c r="D161" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="E161" t="s">
         <v>626</v>
-      </c>
-      <c r="E161" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B162">
         <v>161</v>
@@ -5996,15 +6065,15 @@
         <v>lang$ui(161)</v>
       </c>
       <c r="D162" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E162" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B163">
         <v>162</v>
@@ -6014,15 +6083,15 @@
         <v>lang$ui(162)</v>
       </c>
       <c r="D163" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E163" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B164">
         <v>163</v>
@@ -6032,15 +6101,15 @@
         <v>lang$ui(163)</v>
       </c>
       <c r="D164" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E164" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B165">
         <v>164</v>
@@ -6050,15 +6119,15 @@
         <v>lang$ui(164)</v>
       </c>
       <c r="D165" t="s">
+        <v>629</v>
+      </c>
+      <c r="E165" t="s">
         <v>630</v>
-      </c>
-      <c r="E165" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B166">
         <v>165</v>
@@ -6068,15 +6137,15 @@
         <v>lang$ui(165)</v>
       </c>
       <c r="D166" t="s">
+        <v>631</v>
+      </c>
+      <c r="E166" t="s">
         <v>632</v>
-      </c>
-      <c r="E166" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B167">
         <v>166</v>
@@ -6086,15 +6155,15 @@
         <v>lang$ui(166)</v>
       </c>
       <c r="D167" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E167" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B168">
         <v>167</v>
@@ -6104,10 +6173,10 @@
         <v>lang$ui(167)</v>
       </c>
       <c r="D168" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E168" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -6122,10 +6191,10 @@
         <v>lang$ui(168)</v>
       </c>
       <c r="D169" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E169" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -6140,10 +6209,10 @@
         <v>lang$ui(169)</v>
       </c>
       <c r="D170" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E170" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -6158,15 +6227,15 @@
         <v>lang$ui(170)</v>
       </c>
       <c r="D171" t="s">
+        <v>609</v>
+      </c>
+      <c r="E171" t="s">
         <v>610</v>
-      </c>
-      <c r="E171" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B172">
         <v>171</v>
@@ -6176,15 +6245,15 @@
         <v>lang$ui(171)</v>
       </c>
       <c r="D172" t="s">
+        <v>644</v>
+      </c>
+      <c r="E172" t="s">
         <v>645</v>
-      </c>
-      <c r="E172" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B173">
         <v>172</v>
@@ -6194,15 +6263,15 @@
         <v>lang$ui(172)</v>
       </c>
       <c r="D173" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E173" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B174">
         <v>173</v>
@@ -6212,15 +6281,15 @@
         <v>lang$ui(173)</v>
       </c>
       <c r="D174" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E174" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B175">
         <v>174</v>
@@ -6230,15 +6299,15 @@
         <v>lang$ui(174)</v>
       </c>
       <c r="D175" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E175" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B176">
         <v>175</v>
@@ -6248,15 +6317,15 @@
         <v>lang$ui(175)</v>
       </c>
       <c r="D176" t="s">
+        <v>642</v>
+      </c>
+      <c r="E176" t="s">
         <v>643</v>
-      </c>
-      <c r="E176" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B177">
         <v>176</v>
@@ -6266,10 +6335,10 @@
         <v>lang$ui(176)</v>
       </c>
       <c r="D177" t="s">
+        <v>646</v>
+      </c>
+      <c r="E177" t="s">
         <v>647</v>
-      </c>
-      <c r="E177" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -6284,10 +6353,10 @@
         <v>lang$ui(177)</v>
       </c>
       <c r="D178" t="s">
+        <v>650</v>
+      </c>
+      <c r="E178" t="s">
         <v>651</v>
-      </c>
-      <c r="E178" t="s">
-        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -6315,10 +6384,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -6329,7 +6398,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6339,15 +6408,15 @@
         <v>lang$server(1)</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -6357,15 +6426,15 @@
         <v>lang$server(2)</v>
       </c>
       <c r="D3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -6375,15 +6444,15 @@
         <v>lang$server(3)</v>
       </c>
       <c r="D4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -6393,10 +6462,10 @@
         <v>lang$server(4)</v>
       </c>
       <c r="D5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -6411,10 +6480,10 @@
         <v>lang$server(5)</v>
       </c>
       <c r="D6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -6429,10 +6498,10 @@
         <v>lang$server(6)</v>
       </c>
       <c r="D7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -6447,10 +6516,10 @@
         <v>lang$server(7)</v>
       </c>
       <c r="D8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E8" t="s">
         <v>351</v>
-      </c>
-      <c r="E8" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -6465,10 +6534,10 @@
         <v>lang$server(8)</v>
       </c>
       <c r="D9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -6483,10 +6552,10 @@
         <v>lang$server(9)</v>
       </c>
       <c r="D10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -6501,10 +6570,10 @@
         <v>lang$server(10)</v>
       </c>
       <c r="D11" t="s">
+        <v>358</v>
+      </c>
+      <c r="E11" t="s">
         <v>359</v>
-      </c>
-      <c r="E11" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6519,10 +6588,10 @@
         <v>lang$server(11)</v>
       </c>
       <c r="D12" t="s">
+        <v>361</v>
+      </c>
+      <c r="E12" t="s">
         <v>362</v>
-      </c>
-      <c r="E12" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -6537,10 +6606,10 @@
         <v>lang$server(12)</v>
       </c>
       <c r="D13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -6555,10 +6624,10 @@
         <v>lang$server(13)</v>
       </c>
       <c r="D14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -6573,10 +6642,10 @@
         <v>lang$server(14)</v>
       </c>
       <c r="D15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -6591,10 +6660,10 @@
         <v>lang$server(15)</v>
       </c>
       <c r="D16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E16" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -6609,7 +6678,7 @@
         <v>lang$server(16)</v>
       </c>
       <c r="D17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E17" t="s">
         <v>291</v>
@@ -6627,10 +6696,10 @@
         <v>lang$server(17)</v>
       </c>
       <c r="D18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -6645,10 +6714,10 @@
         <v>lang$server(18)</v>
       </c>
       <c r="D19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -6663,10 +6732,10 @@
         <v>lang$server(19)</v>
       </c>
       <c r="D20" t="s">
+        <v>379</v>
+      </c>
+      <c r="E20" t="s">
         <v>380</v>
-      </c>
-      <c r="E20" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -6681,10 +6750,10 @@
         <v>lang$server(20)</v>
       </c>
       <c r="D21" t="s">
+        <v>381</v>
+      </c>
+      <c r="E21" t="s">
         <v>382</v>
-      </c>
-      <c r="E21" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -6699,10 +6768,10 @@
         <v>lang$server(21)</v>
       </c>
       <c r="D22" t="s">
+        <v>383</v>
+      </c>
+      <c r="E22" t="s">
         <v>384</v>
-      </c>
-      <c r="E22" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -6717,10 +6786,10 @@
         <v>lang$server(22)</v>
       </c>
       <c r="D23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E23" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -6735,10 +6804,10 @@
         <v>lang$server(23)</v>
       </c>
       <c r="D24" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E24" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -6753,10 +6822,10 @@
         <v>lang$server(24)</v>
       </c>
       <c r="D25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -6771,10 +6840,10 @@
         <v>lang$server(25)</v>
       </c>
       <c r="D26" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E26" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -6789,10 +6858,10 @@
         <v>lang$server(26)</v>
       </c>
       <c r="D27" t="s">
+        <v>391</v>
+      </c>
+      <c r="E27" t="s">
         <v>392</v>
-      </c>
-      <c r="E27" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -6807,10 +6876,10 @@
         <v>lang$server(27)</v>
       </c>
       <c r="D28" t="s">
+        <v>393</v>
+      </c>
+      <c r="E28" t="s">
         <v>394</v>
-      </c>
-      <c r="E28" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -6825,10 +6894,10 @@
         <v>lang$server(28)</v>
       </c>
       <c r="D29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -6843,10 +6912,10 @@
         <v>lang$server(29)</v>
       </c>
       <c r="D30" t="s">
+        <v>399</v>
+      </c>
+      <c r="E30" t="s">
         <v>400</v>
-      </c>
-      <c r="E30" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -6861,15 +6930,15 @@
         <v>lang$server(30)</v>
       </c>
       <c r="D31" t="s">
+        <v>401</v>
+      </c>
+      <c r="E31" t="s">
         <v>402</v>
-      </c>
-      <c r="E31" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -6879,15 +6948,15 @@
         <v>lang$server(31)</v>
       </c>
       <c r="D32" t="s">
+        <v>404</v>
+      </c>
+      <c r="E32" t="s">
         <v>405</v>
-      </c>
-      <c r="E32" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -6897,15 +6966,15 @@
         <v>lang$server(32)</v>
       </c>
       <c r="D33" t="s">
+        <v>406</v>
+      </c>
+      <c r="E33" t="s">
         <v>407</v>
-      </c>
-      <c r="E33" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -6915,15 +6984,15 @@
         <v>lang$server(33)</v>
       </c>
       <c r="D34" t="s">
+        <v>408</v>
+      </c>
+      <c r="E34" t="s">
         <v>409</v>
-      </c>
-      <c r="E34" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -6933,15 +7002,15 @@
         <v>lang$server(34)</v>
       </c>
       <c r="D35" t="s">
+        <v>410</v>
+      </c>
+      <c r="E35" t="s">
         <v>411</v>
-      </c>
-      <c r="E35" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -6951,15 +7020,15 @@
         <v>lang$server(35)</v>
       </c>
       <c r="D36" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E36" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -6969,10 +7038,10 @@
         <v>lang$server(36)</v>
       </c>
       <c r="D37" t="s">
+        <v>415</v>
+      </c>
+      <c r="E37" t="s">
         <v>416</v>
-      </c>
-      <c r="E37" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -6987,10 +7056,10 @@
         <v>lang$server(37)</v>
       </c>
       <c r="D38" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -7005,10 +7074,10 @@
         <v>lang$server(38)</v>
       </c>
       <c r="D39" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E39" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -7026,7 +7095,7 @@
         <v>198</v>
       </c>
       <c r="E40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -7059,7 +7128,7 @@
         <v>lang$server(41)</v>
       </c>
       <c r="D42" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E42" t="s">
         <v>134</v>
@@ -7077,10 +7146,10 @@
         <v>lang$server(42)</v>
       </c>
       <c r="D43" t="s">
+        <v>425</v>
+      </c>
+      <c r="E43" t="s">
         <v>426</v>
-      </c>
-      <c r="E43" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -7095,10 +7164,10 @@
         <v>lang$server(43)</v>
       </c>
       <c r="D44" t="s">
+        <v>427</v>
+      </c>
+      <c r="E44" t="s">
         <v>428</v>
-      </c>
-      <c r="E44" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -7113,10 +7182,10 @@
         <v>lang$server(44)</v>
       </c>
       <c r="D45" t="s">
+        <v>429</v>
+      </c>
+      <c r="E45" t="s">
         <v>430</v>
-      </c>
-      <c r="E45" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -7131,10 +7200,10 @@
         <v>lang$server(45)</v>
       </c>
       <c r="D46" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E46" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -7149,10 +7218,10 @@
         <v>lang$server(46)</v>
       </c>
       <c r="D47" t="s">
+        <v>432</v>
+      </c>
+      <c r="E47" t="s">
         <v>433</v>
-      </c>
-      <c r="E47" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -7167,10 +7236,10 @@
         <v>lang$server(47)</v>
       </c>
       <c r="D48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -7185,10 +7254,10 @@
         <v>lang$server(48)</v>
       </c>
       <c r="D49" t="s">
+        <v>435</v>
+      </c>
+      <c r="E49" t="s">
         <v>436</v>
-      </c>
-      <c r="E49" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -7203,10 +7272,10 @@
         <v>lang$server(49)</v>
       </c>
       <c r="D50" t="s">
+        <v>437</v>
+      </c>
+      <c r="E50" t="s">
         <v>438</v>
-      </c>
-      <c r="E50" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -7221,10 +7290,10 @@
         <v>lang$server(50)</v>
       </c>
       <c r="D51" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -7239,10 +7308,10 @@
         <v>lang$server(51)</v>
       </c>
       <c r="D52" t="s">
+        <v>441</v>
+      </c>
+      <c r="E52" t="s">
         <v>442</v>
-      </c>
-      <c r="E52" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -7257,10 +7326,10 @@
         <v>lang$server(52)</v>
       </c>
       <c r="D53" t="s">
+        <v>443</v>
+      </c>
+      <c r="E53" t="s">
         <v>444</v>
-      </c>
-      <c r="E53" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -7275,10 +7344,10 @@
         <v>lang$server(53)</v>
       </c>
       <c r="D54" t="s">
+        <v>445</v>
+      </c>
+      <c r="E54" t="s">
         <v>446</v>
-      </c>
-      <c r="E54" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -7311,10 +7380,10 @@
         <v>lang$server(55)</v>
       </c>
       <c r="D56" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E56" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -7329,10 +7398,10 @@
         <v>lang$server(56)</v>
       </c>
       <c r="D57" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E57" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -7347,7 +7416,7 @@
         <v>lang$server(57)</v>
       </c>
       <c r="D58" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E58" t="s">
         <v>157</v>
@@ -7365,10 +7434,10 @@
         <v>lang$server(58)</v>
       </c>
       <c r="D59" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E59" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -7383,10 +7452,10 @@
         <v>lang$server(59)</v>
       </c>
       <c r="D60" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E60" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -7401,10 +7470,10 @@
         <v>lang$server(60)</v>
       </c>
       <c r="D61" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E61" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -7419,10 +7488,10 @@
         <v>lang$server(61)</v>
       </c>
       <c r="D62" t="s">
+        <v>462</v>
+      </c>
+      <c r="E62" t="s">
         <v>463</v>
-      </c>
-      <c r="E62" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -7437,10 +7506,10 @@
         <v>lang$server(62)</v>
       </c>
       <c r="D63" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E63" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -7458,7 +7527,7 @@
         <v>199</v>
       </c>
       <c r="E64" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -7473,10 +7542,10 @@
         <v>lang$server(64)</v>
       </c>
       <c r="D65" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E65" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -7491,10 +7560,10 @@
         <v>lang$server(65)</v>
       </c>
       <c r="D66" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E66" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -7509,10 +7578,10 @@
         <v>lang$server(66)</v>
       </c>
       <c r="D67" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E67" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -7527,10 +7596,10 @@
         <v>lang$server(67)</v>
       </c>
       <c r="D68" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E68" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -7545,10 +7614,10 @@
         <v>lang$server(68)</v>
       </c>
       <c r="D69" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E69" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -7563,10 +7632,10 @@
         <v>lang$server(69)</v>
       </c>
       <c r="D70" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E70" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -7581,10 +7650,10 @@
         <v>lang$server(70)</v>
       </c>
       <c r="D71" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E71" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -7599,10 +7668,10 @@
         <v>lang$server(71)</v>
       </c>
       <c r="D72" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E72" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -7617,10 +7686,10 @@
         <v>lang$server(72)</v>
       </c>
       <c r="D73" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E73" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -7635,15 +7704,15 @@
         <v>lang$server(73)</v>
       </c>
       <c r="D74" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E74" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -7653,15 +7722,15 @@
         <v>lang$server(74)</v>
       </c>
       <c r="D75" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E75" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -7671,15 +7740,15 @@
         <v>lang$server(75)</v>
       </c>
       <c r="D76" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E76" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -7689,15 +7758,15 @@
         <v>lang$server(76)</v>
       </c>
       <c r="D77" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E77" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -7707,15 +7776,15 @@
         <v>lang$server(77)</v>
       </c>
       <c r="D78" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E78" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -7725,15 +7794,15 @@
         <v>lang$server(78)</v>
       </c>
       <c r="D79" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E79" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -7743,15 +7812,15 @@
         <v>lang$server(79)</v>
       </c>
       <c r="D80" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E80" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -7761,15 +7830,15 @@
         <v>lang$server(80)</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B82">
         <v>81</v>
@@ -7779,15 +7848,15 @@
         <v>lang$server(81)</v>
       </c>
       <c r="D82" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E82" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B83">
         <v>82</v>
@@ -7797,15 +7866,15 @@
         <v>lang$server(82)</v>
       </c>
       <c r="D83" t="s">
+        <v>499</v>
+      </c>
+      <c r="E83" t="s">
         <v>500</v>
-      </c>
-      <c r="E83" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -7815,15 +7884,15 @@
         <v>lang$server(83)</v>
       </c>
       <c r="D84" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E84" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -7833,15 +7902,15 @@
         <v>lang$server(84)</v>
       </c>
       <c r="D85" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E85" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -7851,15 +7920,15 @@
         <v>lang$server(85)</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -7869,15 +7938,15 @@
         <v>lang$server(86)</v>
       </c>
       <c r="D87" t="s">
+        <v>504</v>
+      </c>
+      <c r="E87" s="4" t="s">
         <v>505</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B88">
         <v>87</v>
@@ -7887,15 +7956,15 @@
         <v>lang$server(87)</v>
       </c>
       <c r="D88" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E88" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B89">
         <v>88</v>
@@ -7905,15 +7974,15 @@
         <v>lang$server(88)</v>
       </c>
       <c r="D89" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E89" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -7923,15 +7992,15 @@
         <v>lang$server(89)</v>
       </c>
       <c r="D90" t="s">
+        <v>510</v>
+      </c>
+      <c r="E90" t="s">
         <v>511</v>
-      </c>
-      <c r="E90" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B91">
         <v>90</v>
@@ -7941,15 +8010,15 @@
         <v>lang$server(90)</v>
       </c>
       <c r="D91" t="s">
+        <v>512</v>
+      </c>
+      <c r="E91" t="s">
         <v>513</v>
-      </c>
-      <c r="E91" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -7959,15 +8028,15 @@
         <v>lang$server(91)</v>
       </c>
       <c r="D92" t="s">
+        <v>515</v>
+      </c>
+      <c r="E92" t="s">
         <v>516</v>
-      </c>
-      <c r="E92" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B93">
         <v>92</v>
@@ -7977,15 +8046,15 @@
         <v>lang$server(92)</v>
       </c>
       <c r="D93" t="s">
+        <v>517</v>
+      </c>
+      <c r="E93" t="s">
         <v>518</v>
-      </c>
-      <c r="E93" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B94">
         <v>93</v>
@@ -7995,15 +8064,15 @@
         <v>lang$server(93)</v>
       </c>
       <c r="D94" t="s">
+        <v>519</v>
+      </c>
+      <c r="E94" t="s">
         <v>520</v>
-      </c>
-      <c r="E94" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B95">
         <v>94</v>
@@ -8013,15 +8082,15 @@
         <v>lang$server(94)</v>
       </c>
       <c r="D95" t="s">
+        <v>521</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B96">
         <v>95</v>
@@ -8031,15 +8100,15 @@
         <v>lang$server(95)</v>
       </c>
       <c r="D96" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E96" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B97">
         <v>96</v>
@@ -8049,15 +8118,15 @@
         <v>lang$server(96)</v>
       </c>
       <c r="D97" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B98">
         <v>97</v>
@@ -8067,15 +8136,15 @@
         <v>lang$server(97)</v>
       </c>
       <c r="D98" t="s">
+        <v>527</v>
+      </c>
+      <c r="E98" t="s">
         <v>528</v>
-      </c>
-      <c r="E98" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B99">
         <v>98</v>
@@ -8085,15 +8154,15 @@
         <v>lang$server(98)</v>
       </c>
       <c r="D99" t="s">
+        <v>529</v>
+      </c>
+      <c r="E99" t="s">
         <v>530</v>
-      </c>
-      <c r="E99" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -8103,15 +8172,15 @@
         <v>lang$server(99)</v>
       </c>
       <c r="D100" t="s">
+        <v>531</v>
+      </c>
+      <c r="E100" t="s">
         <v>532</v>
-      </c>
-      <c r="E100" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B101">
         <v>100</v>
@@ -8121,15 +8190,15 @@
         <v>lang$server(100)</v>
       </c>
       <c r="D101" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E101" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B102">
         <v>101</v>
@@ -8139,10 +8208,10 @@
         <v>lang$server(101)</v>
       </c>
       <c r="D102" t="s">
+        <v>534</v>
+      </c>
+      <c r="E102" t="s">
         <v>535</v>
-      </c>
-      <c r="E102" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -8157,10 +8226,10 @@
         <v>lang$server(102)</v>
       </c>
       <c r="D103" t="s">
+        <v>536</v>
+      </c>
+      <c r="E103" t="s">
         <v>537</v>
-      </c>
-      <c r="E103" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -8175,10 +8244,10 @@
         <v>lang$server(103)</v>
       </c>
       <c r="D104" t="s">
+        <v>538</v>
+      </c>
+      <c r="E104" t="s">
         <v>539</v>
-      </c>
-      <c r="E104" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -8193,10 +8262,10 @@
         <v>lang$server(104)</v>
       </c>
       <c r="D105" t="s">
+        <v>540</v>
+      </c>
+      <c r="E105" t="s">
         <v>541</v>
-      </c>
-      <c r="E105" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -8211,7 +8280,7 @@
         <v>lang$server(105)</v>
       </c>
       <c r="D106" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E106" t="s">
         <v>291</v>
@@ -8229,10 +8298,10 @@
         <v>lang$server(106)</v>
       </c>
       <c r="D107" t="s">
+        <v>543</v>
+      </c>
+      <c r="E107" t="s">
         <v>544</v>
-      </c>
-      <c r="E107" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -8247,10 +8316,10 @@
         <v>lang$server(107)</v>
       </c>
       <c r="D108" t="s">
+        <v>545</v>
+      </c>
+      <c r="E108" t="s">
         <v>546</v>
-      </c>
-      <c r="E108" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -8265,10 +8334,10 @@
         <v>lang$server(108)</v>
       </c>
       <c r="D109" t="s">
+        <v>547</v>
+      </c>
+      <c r="E109" t="s">
         <v>548</v>
-      </c>
-      <c r="E109" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -8283,10 +8352,10 @@
         <v>lang$server(109)</v>
       </c>
       <c r="D110" t="s">
+        <v>549</v>
+      </c>
+      <c r="E110" t="s">
         <v>550</v>
-      </c>
-      <c r="E110" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -8301,10 +8370,10 @@
         <v>lang$server(110)</v>
       </c>
       <c r="D111" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E111" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -8319,10 +8388,10 @@
         <v>lang$server(111)</v>
       </c>
       <c r="D112" t="s">
+        <v>555</v>
+      </c>
+      <c r="E112" t="s">
         <v>556</v>
-      </c>
-      <c r="E112" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -8337,10 +8406,10 @@
         <v>lang$server(112)</v>
       </c>
       <c r="D113" t="s">
+        <v>557</v>
+      </c>
+      <c r="E113" t="s">
         <v>558</v>
-      </c>
-      <c r="E113" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -8355,10 +8424,10 @@
         <v>lang$server(113)</v>
       </c>
       <c r="D114" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E114" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -8373,10 +8442,10 @@
         <v>lang$server(114)</v>
       </c>
       <c r="D115" t="s">
+        <v>652</v>
+      </c>
+      <c r="E115" t="s">
         <v>653</v>
-      </c>
-      <c r="E115" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -8391,10 +8460,10 @@
         <v>lang$server(115)</v>
       </c>
       <c r="D116" t="s">
+        <v>560</v>
+      </c>
+      <c r="E116" t="s">
         <v>561</v>
-      </c>
-      <c r="E116" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -8409,10 +8478,10 @@
         <v>lang$server(116)</v>
       </c>
       <c r="D117" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="E117" t="s">
         <v>563</v>
-      </c>
-      <c r="E117" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -8427,10 +8496,10 @@
         <v>lang$server(117)</v>
       </c>
       <c r="D118" t="s">
+        <v>564</v>
+      </c>
+      <c r="E118" t="s">
         <v>565</v>
-      </c>
-      <c r="E118" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -8445,10 +8514,10 @@
         <v>lang$server(118)</v>
       </c>
       <c r="D119" t="s">
+        <v>566</v>
+      </c>
+      <c r="E119" t="s">
         <v>567</v>
-      </c>
-      <c r="E119" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -8463,10 +8532,10 @@
         <v>lang$server(119)</v>
       </c>
       <c r="D120" t="s">
+        <v>568</v>
+      </c>
+      <c r="E120" t="s">
         <v>569</v>
-      </c>
-      <c r="E120" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -8481,10 +8550,10 @@
         <v>lang$server(120)</v>
       </c>
       <c r="D121" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E121" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -8499,10 +8568,10 @@
         <v>lang$server(121)</v>
       </c>
       <c r="D122" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E122" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -8517,10 +8586,10 @@
         <v>lang$server(122)</v>
       </c>
       <c r="D123" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E123" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -8535,10 +8604,10 @@
         <v>lang$server(123)</v>
       </c>
       <c r="D124" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E124" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -8553,10 +8622,10 @@
         <v>lang$server(124)</v>
       </c>
       <c r="D125" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E125" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -8571,10 +8640,10 @@
         <v>lang$server(125)</v>
       </c>
       <c r="D126" t="s">
+        <v>580</v>
+      </c>
+      <c r="E126" t="s">
         <v>581</v>
-      </c>
-      <c r="E126" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -8589,10 +8658,10 @@
         <v>lang$server(126)</v>
       </c>
       <c r="D127" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E127" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -8607,10 +8676,10 @@
         <v>lang$server(127)</v>
       </c>
       <c r="D128" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E128" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -8625,10 +8694,10 @@
         <v>lang$server(128)</v>
       </c>
       <c r="D129" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E129" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -8643,10 +8712,10 @@
         <v>lang$server(129)</v>
       </c>
       <c r="D130" t="s">
+        <v>588</v>
+      </c>
+      <c r="E130" t="s">
         <v>589</v>
-      </c>
-      <c r="E130" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -8661,10 +8730,10 @@
         <v>lang$server(130)</v>
       </c>
       <c r="D131" t="s">
+        <v>599</v>
+      </c>
+      <c r="E131" t="s">
         <v>600</v>
-      </c>
-      <c r="E131" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -8679,10 +8748,10 @@
         <v>lang$server(131)</v>
       </c>
       <c r="D132" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E132" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -8697,10 +8766,10 @@
         <v>lang$server(132)</v>
       </c>
       <c r="D133" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E133" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -8715,10 +8784,10 @@
         <v>lang$server(133)</v>
       </c>
       <c r="D134" t="s">
+        <v>621</v>
+      </c>
+      <c r="E134" t="s">
         <v>622</v>
-      </c>
-      <c r="E134" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -8733,10 +8802,10 @@
         <v>lang$server(134)</v>
       </c>
       <c r="D135" t="s">
+        <v>613</v>
+      </c>
+      <c r="E135" t="s">
         <v>614</v>
-      </c>
-      <c r="E135" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -8751,10 +8820,10 @@
         <v>lang$server(135)</v>
       </c>
       <c r="D136" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E136" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the behaviour of the download button, so that data preparation and actual download are separated into two steps
</commit_message>
<xml_diff>
--- a/data-raw/languages.xlsx
+++ b/data-raw/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Gremienarbeit/TWA/Projekte/Spectran/Spectran/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039E9377-188E-9E4F-905F-E812145FAD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FC1F23-173C-E440-AE20-C36BD38942DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11680" yWindow="3040" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
+    <workbookView xWindow="5760" yWindow="3040" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="664">
   <si>
     <t>Deutsch</t>
   </si>
@@ -1996,12 +1996,6 @@
     <t>adjusted</t>
   </si>
   <si>
-    <t>Der Export wurde erfolgreich abgeschlossen.</t>
-  </si>
-  <si>
-    <t>Export was successful.</t>
-  </si>
-  <si>
     <t>Header</t>
   </si>
   <si>
@@ -2024,6 +2018,18 @@
   </si>
   <si>
     <t xml:space="preserve"> section. Display options from that tab are kept for the export. For a few exceptions, export options can be overritten in the </t>
+  </si>
+  <si>
+    <t>Erstelle ZIP-Datei</t>
+  </si>
+  <si>
+    <t>Create ZIP file</t>
+  </si>
+  <si>
+    <t>Export file was successfully created. It can be downloaded now:</t>
+  </si>
+  <si>
+    <t>Die Exportdatei wurde erfolgreich vorbereitet und kann nun heruntergeladen werden:</t>
   </si>
 </sst>
 </file>
@@ -2620,7 +2626,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2630,15 +2636,15 @@
         <v>lang$global(12)</v>
       </c>
       <c r="D13" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E13" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2648,15 +2654,15 @@
         <v>lang$global(13)</v>
       </c>
       <c r="D14" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E14" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -2666,10 +2672,10 @@
         <v>lang$global(14)</v>
       </c>
       <c r="D15" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E15" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3143,7 +3149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16C6AC7-F954-EC4A-BACE-CEC04494FD73}">
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+    <sheetView topLeftCell="A105" workbookViewId="0">
       <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
@@ -5438,7 +5444,7 @@
         <v>263</v>
       </c>
       <c r="E127" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -6366,10 +6372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496328DD-5C8E-3D45-AB81-313F176488D7}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8442,10 +8448,10 @@
         <v>lang$server(114)</v>
       </c>
       <c r="D115" t="s">
-        <v>652</v>
+        <v>663</v>
       </c>
       <c r="E115" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -8726,7 +8732,7 @@
         <v>130</v>
       </c>
       <c r="C131" s="3" t="str">
-        <f t="shared" ref="C131:C135" si="2">"lang$server(" &amp; B131 &amp; ")"</f>
+        <f t="shared" ref="C131:C137" si="2">"lang$server(" &amp; B131 &amp; ")"</f>
         <v>lang$server(130)</v>
       </c>
       <c r="D131" t="s">
@@ -8824,6 +8830,24 @@
       </c>
       <c r="E136" t="s">
         <v>648</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>259</v>
+      </c>
+      <c r="B137">
+        <v>136</v>
+      </c>
+      <c r="C137" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>lang$server(136)</v>
+      </c>
+      <c r="D137" t="s">
+        <v>660</v>
+      </c>
+      <c r="E137" t="s">
+        <v>661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the tutorial and changed notification messages
</commit_message>
<xml_diff>
--- a/data-raw/languages.xlsx
+++ b/data-raw/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Gremienarbeit/TWA/Projekte/Spectran/Spectran/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FC1F23-173C-E440-AE20-C36BD38942DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C02E8D-8425-F64E-A2BE-A9BDD4597F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3040" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
+    <workbookView xWindow="51200" yWindow="15120" windowWidth="18760" windowHeight="18880" activeTab="2" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="659">
   <si>
     <t>Deutsch</t>
   </si>
@@ -1042,30 +1042,9 @@
     <t>Verwendete Pakete in R:</t>
   </si>
   <si>
-    <t>https://mstream.hm.edu/static/mh_default_org/api/fc28fe08-8633-4457-bdd4-8fb23cc93b22/701f69b3-4c42-4dbd-9d2e-ecbc8c8843bf/concat.mp4</t>
-  </si>
-  <si>
-    <t>https://mstream.hm.edu/static/mh_default_org/api/e7e1bce6-baa7-4398-9868-2cd3e60fe6d1/0264a242-2421-4efd-8910-baa697cb3a76/concat.mp4</t>
-  </si>
-  <si>
     <t>Tutorial_Kurz</t>
   </si>
   <si>
-    <t>Tutorial_1</t>
-  </si>
-  <si>
-    <t>Tutorial_2</t>
-  </si>
-  <si>
-    <t>Tutorial_3</t>
-  </si>
-  <si>
-    <t>https://mstream.hm.edu/static/mh_default_org/api/afd5206c-d94a-4e42-b692-d5f169b5e8a6/451737a4-fa44-4cbd-a075-51c333feac70/concat.mp4</t>
-  </si>
-  <si>
-    <t>https://mstream.hm.edu/static/mh_default_org/api/44110ec1-1533-41c7-9085-ee30caf80458/beb097cb-a757-43e4-be49-64710d23c3bb/concat.mp4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gültige Spalten: 1 bis </t>
   </si>
   <si>
@@ -2030,6 +2009,12 @@
   </si>
   <si>
     <t>Die Exportdatei wurde erfolgreich vorbereitet und kann nun heruntergeladen werden:</t>
+  </si>
+  <si>
+    <t>https://mstream.hm.edu/static/mh_default_org/api/eba0e91a-856c-4bde-98e4-dbed166a8581/09ecbc0b-14f9-4277-bd3e-15fa52bcd5cf/concat.mp4</t>
+  </si>
+  <si>
+    <t>https://mstream.hm.edu/static/mh_default_org/api/4ea1066d-53d9-4461-a4e2-665fadbf1312/8ee8c531-9b35-4896-baab-f87670b7a916/concat.mp4</t>
   </si>
 </sst>
 </file>
@@ -2414,10 +2399,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="C1" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2531,7 +2516,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2549,7 +2534,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2567,7 +2552,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2585,7 +2570,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2603,7 +2588,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2621,12 +2606,12 @@
         <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2636,15 +2621,15 @@
         <v>lang$global(12)</v>
       </c>
       <c r="D13" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="E13" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2654,15 +2639,15 @@
         <v>lang$global(13)</v>
       </c>
       <c r="D14" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="E14" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -2672,10 +2657,10 @@
         <v>lang$global(14)</v>
       </c>
       <c r="D15" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="E15" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3149,7 +3134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16C6AC7-F954-EC4A-BACE-CEC04494FD73}">
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
@@ -3167,10 +3152,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="C1" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3299,7 +3284,7 @@
         <v>lang$ui(7)</v>
       </c>
       <c r="D8" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
@@ -3662,7 +3647,7 @@
         <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3767,10 +3752,10 @@
         <v>lang$ui(33)</v>
       </c>
       <c r="D34" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="E34" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -4040,7 +4025,7 @@
         <v>114</v>
       </c>
       <c r="E49" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -4055,10 +4040,10 @@
         <v>lang$ui(49)</v>
       </c>
       <c r="D50" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="E50" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -4073,10 +4058,10 @@
         <v>lang$ui(50)</v>
       </c>
       <c r="D51" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="E51" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -4325,10 +4310,10 @@
         <v>lang$ui(64)</v>
       </c>
       <c r="D65" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="E65" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4379,10 +4364,10 @@
         <v>lang$ui(67)</v>
       </c>
       <c r="D68" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="E68" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -4397,10 +4382,10 @@
         <v>lang$ui(68)</v>
       </c>
       <c r="D69" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="E69" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4703,10 +4688,10 @@
         <v>lang$ui(85)</v>
       </c>
       <c r="D86" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E86" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -4721,10 +4706,10 @@
         <v>lang$ui(86)</v>
       </c>
       <c r="D87" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="E87" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -4919,7 +4904,7 @@
         <v>lang$ui(97)</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>212</v>
@@ -5081,7 +5066,7 @@
         <v>lang$ui(106)</v>
       </c>
       <c r="D107" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="E107" t="s">
         <v>248</v>
@@ -5444,7 +5429,7 @@
         <v>263</v>
       </c>
       <c r="E127" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -6035,10 +6020,10 @@
         <v>lang$ui(159)</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="E160" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6053,10 +6038,10 @@
         <v>lang$ui(160)</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="E161" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -6071,10 +6056,10 @@
         <v>lang$ui(161)</v>
       </c>
       <c r="D162" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="E162" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -6089,10 +6074,10 @@
         <v>lang$ui(162)</v>
       </c>
       <c r="D163" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="E163" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -6107,10 +6092,10 @@
         <v>lang$ui(163)</v>
       </c>
       <c r="D164" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="E164" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -6125,10 +6110,10 @@
         <v>lang$ui(164)</v>
       </c>
       <c r="D165" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="E165" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -6143,10 +6128,10 @@
         <v>lang$ui(165)</v>
       </c>
       <c r="D166" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="E166" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -6197,10 +6182,10 @@
         <v>lang$ui(168)</v>
       </c>
       <c r="D169" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="E169" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -6215,10 +6200,10 @@
         <v>lang$ui(169)</v>
       </c>
       <c r="D170" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="E170" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -6233,10 +6218,10 @@
         <v>lang$ui(170)</v>
       </c>
       <c r="D171" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="E171" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -6251,10 +6236,10 @@
         <v>lang$ui(171)</v>
       </c>
       <c r="D172" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="E172" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -6269,10 +6254,10 @@
         <v>lang$ui(172)</v>
       </c>
       <c r="D173" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E173" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -6287,10 +6272,10 @@
         <v>lang$ui(173)</v>
       </c>
       <c r="D174" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="E174" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -6305,10 +6290,10 @@
         <v>lang$ui(174)</v>
       </c>
       <c r="D175" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="E175" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -6323,10 +6308,10 @@
         <v>lang$ui(175)</v>
       </c>
       <c r="D176" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="E176" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -6341,10 +6326,10 @@
         <v>lang$ui(176)</v>
       </c>
       <c r="D177" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="E177" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -6359,10 +6344,10 @@
         <v>lang$ui(177)</v>
       </c>
       <c r="D178" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="E178" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -6374,8 +6359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496328DD-5C8E-3D45-AB81-313F176488D7}">
   <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6390,10 +6375,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="C1" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -6404,7 +6389,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6414,16 +6399,13 @@
         <v>lang$server(1)</v>
       </c>
       <c r="D2" t="s">
-        <v>334</v>
+        <v>658</v>
       </c>
       <c r="E2" t="s">
-        <v>334</v>
+        <v>657</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>337</v>
-      </c>
       <c r="B3">
         <v>2</v>
       </c>
@@ -6431,17 +6413,8 @@
         <f t="shared" ref="C3:C66" si="0">"lang$server(" &amp; B3 &amp; ")"</f>
         <v>lang$server(2)</v>
       </c>
-      <c r="D3" t="s">
-        <v>335</v>
-      </c>
-      <c r="E3" t="s">
-        <v>335</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>338</v>
-      </c>
       <c r="B4">
         <v>3</v>
       </c>
@@ -6449,29 +6422,14 @@
         <f t="shared" si="0"/>
         <v>lang$server(3)</v>
       </c>
-      <c r="D4" t="s">
-        <v>340</v>
-      </c>
-      <c r="E4" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>339</v>
-      </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>lang$server(4)</v>
-      </c>
-      <c r="D5" t="s">
-        <v>341</v>
-      </c>
-      <c r="E5" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -6486,10 +6444,10 @@
         <v>lang$server(5)</v>
       </c>
       <c r="D6" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="E6" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -6504,10 +6462,10 @@
         <v>lang$server(6)</v>
       </c>
       <c r="D7" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E7" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -6522,10 +6480,10 @@
         <v>lang$server(7)</v>
       </c>
       <c r="D8" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="E8" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -6540,10 +6498,10 @@
         <v>lang$server(8)</v>
       </c>
       <c r="D9" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E9" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -6558,10 +6516,10 @@
         <v>lang$server(9)</v>
       </c>
       <c r="D10" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="E10" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -6576,10 +6534,10 @@
         <v>lang$server(10)</v>
       </c>
       <c r="D11" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E11" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6594,10 +6552,10 @@
         <v>lang$server(11)</v>
       </c>
       <c r="D12" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="E12" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -6612,10 +6570,10 @@
         <v>lang$server(12)</v>
       </c>
       <c r="D13" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E13" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -6630,10 +6588,10 @@
         <v>lang$server(13)</v>
       </c>
       <c r="D14" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="E14" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -6648,10 +6606,10 @@
         <v>lang$server(14)</v>
       </c>
       <c r="D15" t="s">
+        <v>342</v>
+      </c>
+      <c r="E15" t="s">
         <v>349</v>
-      </c>
-      <c r="E15" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -6666,10 +6624,10 @@
         <v>lang$server(15)</v>
       </c>
       <c r="D16" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="E16" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -6684,7 +6642,7 @@
         <v>lang$server(16)</v>
       </c>
       <c r="D17" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="E17" t="s">
         <v>291</v>
@@ -6702,10 +6660,10 @@
         <v>lang$server(17)</v>
       </c>
       <c r="D18" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="E18" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -6720,10 +6678,10 @@
         <v>lang$server(18)</v>
       </c>
       <c r="D19" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="E19" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -6738,10 +6696,10 @@
         <v>lang$server(19)</v>
       </c>
       <c r="D20" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="E20" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -6756,10 +6714,10 @@
         <v>lang$server(20)</v>
       </c>
       <c r="D21" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E21" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -6774,10 +6732,10 @@
         <v>lang$server(21)</v>
       </c>
       <c r="D22" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="E22" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -6792,10 +6750,10 @@
         <v>lang$server(22)</v>
       </c>
       <c r="D23" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="E23" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -6810,10 +6768,10 @@
         <v>lang$server(23)</v>
       </c>
       <c r="D24" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="E24" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -6828,10 +6786,10 @@
         <v>lang$server(24)</v>
       </c>
       <c r="D25" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="E25" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -6846,10 +6804,10 @@
         <v>lang$server(25)</v>
       </c>
       <c r="D26" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="E26" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -6864,10 +6822,10 @@
         <v>lang$server(26)</v>
       </c>
       <c r="D27" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="E27" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -6882,10 +6840,10 @@
         <v>lang$server(27)</v>
       </c>
       <c r="D28" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E28" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -6900,10 +6858,10 @@
         <v>lang$server(28)</v>
       </c>
       <c r="D29" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="E29" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -6918,10 +6876,10 @@
         <v>lang$server(29)</v>
       </c>
       <c r="D30" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E30" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -6936,15 +6894,15 @@
         <v>lang$server(30)</v>
       </c>
       <c r="D31" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="E31" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -6954,15 +6912,15 @@
         <v>lang$server(31)</v>
       </c>
       <c r="D32" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E32" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -6972,15 +6930,15 @@
         <v>lang$server(32)</v>
       </c>
       <c r="D33" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="E33" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -6990,15 +6948,15 @@
         <v>lang$server(33)</v>
       </c>
       <c r="D34" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="E34" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -7008,15 +6966,15 @@
         <v>lang$server(34)</v>
       </c>
       <c r="D35" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="E35" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -7026,15 +6984,15 @@
         <v>lang$server(35)</v>
       </c>
       <c r="D36" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="E36" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -7044,10 +7002,10 @@
         <v>lang$server(36)</v>
       </c>
       <c r="D37" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="E37" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -7062,10 +7020,10 @@
         <v>lang$server(37)</v>
       </c>
       <c r="D38" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="E38" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -7080,10 +7038,10 @@
         <v>lang$server(38)</v>
       </c>
       <c r="D39" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="E39" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -7101,7 +7059,7 @@
         <v>198</v>
       </c>
       <c r="E40" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -7134,7 +7092,7 @@
         <v>lang$server(41)</v>
       </c>
       <c r="D42" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="E42" t="s">
         <v>134</v>
@@ -7152,10 +7110,10 @@
         <v>lang$server(42)</v>
       </c>
       <c r="D43" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="E43" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -7170,10 +7128,10 @@
         <v>lang$server(43)</v>
       </c>
       <c r="D44" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="E44" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -7188,10 +7146,10 @@
         <v>lang$server(44)</v>
       </c>
       <c r="D45" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="E45" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -7206,10 +7164,10 @@
         <v>lang$server(45)</v>
       </c>
       <c r="D46" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="E46" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -7224,10 +7182,10 @@
         <v>lang$server(46)</v>
       </c>
       <c r="D47" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="E47" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -7242,10 +7200,10 @@
         <v>lang$server(47)</v>
       </c>
       <c r="D48" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E48" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -7260,10 +7218,10 @@
         <v>lang$server(48)</v>
       </c>
       <c r="D49" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="E49" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -7278,10 +7236,10 @@
         <v>lang$server(49)</v>
       </c>
       <c r="D50" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="E50" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -7296,10 +7254,10 @@
         <v>lang$server(50)</v>
       </c>
       <c r="D51" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="E51" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -7314,10 +7272,10 @@
         <v>lang$server(51)</v>
       </c>
       <c r="D52" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="E52" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -7332,10 +7290,10 @@
         <v>lang$server(52)</v>
       </c>
       <c r="D53" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="E53" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -7350,10 +7308,10 @@
         <v>lang$server(53)</v>
       </c>
       <c r="D54" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="E54" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -7386,10 +7344,10 @@
         <v>lang$server(55)</v>
       </c>
       <c r="D56" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="E56" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -7404,10 +7362,10 @@
         <v>lang$server(56)</v>
       </c>
       <c r="D57" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="E57" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -7422,7 +7380,7 @@
         <v>lang$server(57)</v>
       </c>
       <c r="D58" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="E58" t="s">
         <v>157</v>
@@ -7440,10 +7398,10 @@
         <v>lang$server(58)</v>
       </c>
       <c r="D59" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="E59" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -7458,10 +7416,10 @@
         <v>lang$server(59)</v>
       </c>
       <c r="D60" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="E60" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -7476,10 +7434,10 @@
         <v>lang$server(60)</v>
       </c>
       <c r="D61" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="E61" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -7494,10 +7452,10 @@
         <v>lang$server(61)</v>
       </c>
       <c r="D62" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="E62" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -7512,10 +7470,10 @@
         <v>lang$server(62)</v>
       </c>
       <c r="D63" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="E63" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -7533,7 +7491,7 @@
         <v>199</v>
       </c>
       <c r="E64" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -7548,10 +7506,10 @@
         <v>lang$server(64)</v>
       </c>
       <c r="D65" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="E65" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -7566,10 +7524,10 @@
         <v>lang$server(65)</v>
       </c>
       <c r="D66" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="E66" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -7584,10 +7542,10 @@
         <v>lang$server(66)</v>
       </c>
       <c r="D67" t="s">
+        <v>459</v>
+      </c>
+      <c r="E67" t="s">
         <v>466</v>
-      </c>
-      <c r="E67" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -7602,10 +7560,10 @@
         <v>lang$server(67)</v>
       </c>
       <c r="D68" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="E68" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -7620,10 +7578,10 @@
         <v>lang$server(68)</v>
       </c>
       <c r="D69" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E69" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -7638,10 +7596,10 @@
         <v>lang$server(69)</v>
       </c>
       <c r="D70" t="s">
+        <v>462</v>
+      </c>
+      <c r="E70" t="s">
         <v>469</v>
-      </c>
-      <c r="E70" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -7656,10 +7614,10 @@
         <v>lang$server(70)</v>
       </c>
       <c r="D71" t="s">
+        <v>463</v>
+      </c>
+      <c r="E71" t="s">
         <v>470</v>
-      </c>
-      <c r="E71" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -7674,10 +7632,10 @@
         <v>lang$server(71)</v>
       </c>
       <c r="D72" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="E72" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -7692,10 +7650,10 @@
         <v>lang$server(72)</v>
       </c>
       <c r="D73" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="E73" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -7710,15 +7668,15 @@
         <v>lang$server(73)</v>
       </c>
       <c r="D74" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="E74" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -7728,15 +7686,15 @@
         <v>lang$server(74)</v>
       </c>
       <c r="D75" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="E75" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -7746,15 +7704,15 @@
         <v>lang$server(75)</v>
       </c>
       <c r="D76" t="s">
+        <v>479</v>
+      </c>
+      <c r="E76" t="s">
         <v>486</v>
-      </c>
-      <c r="E76" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -7764,15 +7722,15 @@
         <v>lang$server(76)</v>
       </c>
       <c r="D77" t="s">
+        <v>480</v>
+      </c>
+      <c r="E77" t="s">
         <v>487</v>
-      </c>
-      <c r="E77" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -7782,15 +7740,15 @@
         <v>lang$server(77)</v>
       </c>
       <c r="D78" t="s">
+        <v>481</v>
+      </c>
+      <c r="E78" t="s">
         <v>488</v>
-      </c>
-      <c r="E78" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -7800,15 +7758,15 @@
         <v>lang$server(78)</v>
       </c>
       <c r="D79" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="E79" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -7818,15 +7776,15 @@
         <v>lang$server(79)</v>
       </c>
       <c r="D80" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="E80" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -7836,15 +7794,15 @@
         <v>lang$server(80)</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B82">
         <v>81</v>
@@ -7854,15 +7812,15 @@
         <v>lang$server(81)</v>
       </c>
       <c r="D82" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="E82" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B83">
         <v>82</v>
@@ -7872,15 +7830,15 @@
         <v>lang$server(82)</v>
       </c>
       <c r="D83" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="E83" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -7890,15 +7848,15 @@
         <v>lang$server(83)</v>
       </c>
       <c r="D84" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="E84" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -7908,15 +7866,15 @@
         <v>lang$server(84)</v>
       </c>
       <c r="D85" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="E85" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -7926,15 +7884,15 @@
         <v>lang$server(85)</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -7944,15 +7902,15 @@
         <v>lang$server(86)</v>
       </c>
       <c r="D87" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B88">
         <v>87</v>
@@ -7962,15 +7920,15 @@
         <v>lang$server(87)</v>
       </c>
       <c r="D88" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="E88" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B89">
         <v>88</v>
@@ -7980,15 +7938,15 @@
         <v>lang$server(88)</v>
       </c>
       <c r="D89" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="E89" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -7998,15 +7956,15 @@
         <v>lang$server(89)</v>
       </c>
       <c r="D90" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="E90" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B91">
         <v>90</v>
@@ -8016,15 +7974,15 @@
         <v>lang$server(90)</v>
       </c>
       <c r="D91" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="E91" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -8034,15 +7992,15 @@
         <v>lang$server(91)</v>
       </c>
       <c r="D92" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="E92" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B93">
         <v>92</v>
@@ -8052,15 +8010,15 @@
         <v>lang$server(92)</v>
       </c>
       <c r="D93" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="E93" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B94">
         <v>93</v>
@@ -8070,15 +8028,15 @@
         <v>lang$server(93)</v>
       </c>
       <c r="D94" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="E94" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B95">
         <v>94</v>
@@ -8088,15 +8046,15 @@
         <v>lang$server(94)</v>
       </c>
       <c r="D95" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B96">
         <v>95</v>
@@ -8106,15 +8064,15 @@
         <v>lang$server(95)</v>
       </c>
       <c r="D96" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="E96" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B97">
         <v>96</v>
@@ -8124,15 +8082,15 @@
         <v>lang$server(96)</v>
       </c>
       <c r="D97" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B98">
         <v>97</v>
@@ -8142,15 +8100,15 @@
         <v>lang$server(97)</v>
       </c>
       <c r="D98" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="E98" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B99">
         <v>98</v>
@@ -8160,15 +8118,15 @@
         <v>lang$server(98)</v>
       </c>
       <c r="D99" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="E99" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -8178,15 +8136,15 @@
         <v>lang$server(99)</v>
       </c>
       <c r="D100" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="E100" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B101">
         <v>100</v>
@@ -8196,15 +8154,15 @@
         <v>lang$server(100)</v>
       </c>
       <c r="D101" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="E101" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B102">
         <v>101</v>
@@ -8214,10 +8172,10 @@
         <v>lang$server(101)</v>
       </c>
       <c r="D102" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="E102" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -8232,10 +8190,10 @@
         <v>lang$server(102)</v>
       </c>
       <c r="D103" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="E103" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -8250,10 +8208,10 @@
         <v>lang$server(103)</v>
       </c>
       <c r="D104" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="E104" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -8268,10 +8226,10 @@
         <v>lang$server(104)</v>
       </c>
       <c r="D105" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="E105" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -8286,7 +8244,7 @@
         <v>lang$server(105)</v>
       </c>
       <c r="D106" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="E106" t="s">
         <v>291</v>
@@ -8304,10 +8262,10 @@
         <v>lang$server(106)</v>
       </c>
       <c r="D107" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="E107" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -8322,10 +8280,10 @@
         <v>lang$server(107)</v>
       </c>
       <c r="D108" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="E108" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -8340,10 +8298,10 @@
         <v>lang$server(108)</v>
       </c>
       <c r="D109" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="E109" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -8358,10 +8316,10 @@
         <v>lang$server(109)</v>
       </c>
       <c r="D110" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="E110" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -8376,10 +8334,10 @@
         <v>lang$server(110)</v>
       </c>
       <c r="D111" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="E111" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -8394,10 +8352,10 @@
         <v>lang$server(111)</v>
       </c>
       <c r="D112" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="E112" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -8412,10 +8370,10 @@
         <v>lang$server(112)</v>
       </c>
       <c r="D113" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="E113" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -8430,10 +8388,10 @@
         <v>lang$server(113)</v>
       </c>
       <c r="D114" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="E114" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -8448,10 +8406,10 @@
         <v>lang$server(114)</v>
       </c>
       <c r="D115" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="E115" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -8466,10 +8424,10 @@
         <v>lang$server(115)</v>
       </c>
       <c r="D116" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="E116" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -8484,10 +8442,10 @@
         <v>lang$server(116)</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="E117" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -8502,10 +8460,10 @@
         <v>lang$server(117)</v>
       </c>
       <c r="D118" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="E118" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -8520,10 +8478,10 @@
         <v>lang$server(118)</v>
       </c>
       <c r="D119" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="E119" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -8538,10 +8496,10 @@
         <v>lang$server(119)</v>
       </c>
       <c r="D120" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="E120" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -8556,10 +8514,10 @@
         <v>lang$server(120)</v>
       </c>
       <c r="D121" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="E121" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -8574,10 +8532,10 @@
         <v>lang$server(121)</v>
       </c>
       <c r="D122" t="s">
+        <v>564</v>
+      </c>
+      <c r="E122" t="s">
         <v>571</v>
-      </c>
-      <c r="E122" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -8592,10 +8550,10 @@
         <v>lang$server(122)</v>
       </c>
       <c r="D123" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="E123" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -8610,10 +8568,10 @@
         <v>lang$server(123)</v>
       </c>
       <c r="D124" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="E124" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -8628,10 +8586,10 @@
         <v>lang$server(124)</v>
       </c>
       <c r="D125" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="E125" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -8646,10 +8604,10 @@
         <v>lang$server(125)</v>
       </c>
       <c r="D126" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="E126" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -8664,10 +8622,10 @@
         <v>lang$server(126)</v>
       </c>
       <c r="D127" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="E127" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -8682,10 +8640,10 @@
         <v>lang$server(127)</v>
       </c>
       <c r="D128" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="E128" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -8700,10 +8658,10 @@
         <v>lang$server(128)</v>
       </c>
       <c r="D129" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="E129" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -8718,10 +8676,10 @@
         <v>lang$server(129)</v>
       </c>
       <c r="D130" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="E130" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -8736,10 +8694,10 @@
         <v>lang$server(130)</v>
       </c>
       <c r="D131" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="E131" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -8754,10 +8712,10 @@
         <v>lang$server(131)</v>
       </c>
       <c r="D132" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="E132" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -8772,10 +8730,10 @@
         <v>lang$server(132)</v>
       </c>
       <c r="D133" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="E133" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -8790,10 +8748,10 @@
         <v>lang$server(133)</v>
       </c>
       <c r="D134" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="E134" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -8808,10 +8766,10 @@
         <v>lang$server(134)</v>
       </c>
       <c r="D135" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="E135" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -8826,10 +8784,10 @@
         <v>lang$server(135)</v>
       </c>
       <c r="D136" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="E136" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -8844,10 +8802,10 @@
         <v>lang$server(136)</v>
       </c>
       <c r="D137" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="E137" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing the LiTG full name to reflect the name change
</commit_message>
<xml_diff>
--- a/data-raw/languages.xlsx
+++ b/data-raw/languages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Gremienarbeit/TWA/Projekte/Spectran/Spectran/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951C3440-D81A-5E4C-9294-61F5F623A96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D19B870-C999-AE41-8B53-C41A681CDB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="2980" windowWidth="29280" windowHeight="21840" activeTab="1" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
+    <workbookView xWindow="7200" yWindow="2600" windowWidth="29280" windowHeight="21840" activeTab="1" xr2:uid="{910D35BB-F26F-9249-A4C4-73C92B270189}"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="1" r:id="rId1"/>
@@ -1846,18 +1846,9 @@
     <t>Autor:</t>
   </si>
   <si>
-    <t>This application is a publication of the German technical lighting society.</t>
-  </si>
-  <si>
     <t>Author:</t>
   </si>
   <si>
-    <t>Diese Applikation ist eine Veröffentlichung der Deutschen Lichttechnischen Gesellschaft e.V..</t>
-  </si>
-  <si>
-    <t>Deutsche Lichttechnische Gesellschaft e.V. (LiTG)</t>
-  </si>
-  <si>
     <t>Danneckerstraße 16</t>
   </si>
   <si>
@@ -2084,6 +2075,15 @@
   </si>
   <si>
     <t>In den folgenden Abschnitten werden einige Funktionen der App dargestellt. Aus Speichergründen sind die Beispielbilder lediglich in einer Sprache (Englisch) dargestellt. Die Applikation selbst ist jedoch vollständig übersetzt. Weiter unten haben Sie Zugriff auf ein Tutorial Video.</t>
+  </si>
+  <si>
+    <t>Deutsche Gesellschaft für LichtTechnik und LichtGestaltung e.V.</t>
+  </si>
+  <si>
+    <t>Diese Applikation ist eine Veröffentlichung der Deutsche Gesellschaft für LichtTechnik und LichtGestaltung e.V..</t>
+  </si>
+  <si>
+    <t>This application is a publication of the German Society for Lighting Design and Lighting Technology (LiTG)</t>
   </si>
 </sst>
 </file>
@@ -2152,9 +2152,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2192,7 +2192,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2298,7 +2298,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2440,7 +2440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2451,7 +2451,7 @@
   <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2510,10 +2510,10 @@
         <v>lang$global(2)</v>
       </c>
       <c r="D3" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="E3" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2528,10 +2528,10 @@
         <v>lang$global(3)</v>
       </c>
       <c r="D4" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E4" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2546,10 +2546,10 @@
         <v>lang$global(4)</v>
       </c>
       <c r="D5" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E5" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2582,10 +2582,10 @@
         <v>lang$global(6)</v>
       </c>
       <c r="D7" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E7" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2600,10 +2600,10 @@
         <v>lang$global(7)</v>
       </c>
       <c r="D8" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="E8" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2618,10 +2618,10 @@
         <v>lang$global(8)</v>
       </c>
       <c r="D9" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="E9" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2636,10 +2636,10 @@
         <v>lang$global(9)</v>
       </c>
       <c r="D10" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="E10" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2654,10 +2654,10 @@
         <v>lang$global(10)</v>
       </c>
       <c r="D11" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="E11" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2680,7 +2680,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2690,15 +2690,15 @@
         <v>lang$global(12)</v>
       </c>
       <c r="D13" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E13" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2708,15 +2708,15 @@
         <v>lang$global(13)</v>
       </c>
       <c r="D14" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="E14" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -2726,10 +2726,10 @@
         <v>lang$global(14)</v>
       </c>
       <c r="D15" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E15" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3203,8 +3203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16C6AC7-F954-EC4A-BACE-CEC04494FD73}">
   <dimension ref="A1:E189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3533,7 +3533,7 @@
         <v>lang$ui(17)</v>
       </c>
       <c r="D18" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E18" t="s">
         <v>39</v>
@@ -5153,10 +5153,10 @@
         <v>lang$ui(107)</v>
       </c>
       <c r="D108" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="E108" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -5498,7 +5498,7 @@
         <v>249</v>
       </c>
       <c r="E127" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -6053,10 +6053,10 @@
         <v>lang$ui(157)</v>
       </c>
       <c r="D158" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="E158" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -6143,10 +6143,10 @@
         <v>lang$ui(162)</v>
       </c>
       <c r="D163" t="s">
-        <v>604</v>
+        <v>680</v>
       </c>
       <c r="E163" t="s">
-        <v>602</v>
+        <v>681</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -6164,7 +6164,7 @@
         <v>601</v>
       </c>
       <c r="E164" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -6305,10 +6305,10 @@
         <v>lang$ui(171)</v>
       </c>
       <c r="D172" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E172" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -6323,10 +6323,10 @@
         <v>lang$ui(172)</v>
       </c>
       <c r="D173" t="s">
-        <v>605</v>
+        <v>679</v>
       </c>
       <c r="E173" t="s">
-        <v>605</v>
+        <v>679</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -6341,10 +6341,10 @@
         <v>lang$ui(173)</v>
       </c>
       <c r="D174" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E174" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -6359,10 +6359,10 @@
         <v>lang$ui(174)</v>
       </c>
       <c r="D175" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E175" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -6377,10 +6377,10 @@
         <v>lang$ui(175)</v>
       </c>
       <c r="D176" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E176" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -6395,10 +6395,10 @@
         <v>lang$ui(176)</v>
       </c>
       <c r="D177" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E177" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -6413,10 +6413,10 @@
         <v>lang$ui(177)</v>
       </c>
       <c r="D178" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E178" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -6431,10 +6431,10 @@
         <v>lang$ui(178)</v>
       </c>
       <c r="D179" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E179" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -6449,10 +6449,10 @@
         <v>lang$ui(179)</v>
       </c>
       <c r="D180" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E180" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -6467,10 +6467,10 @@
         <v>lang$ui(180)</v>
       </c>
       <c r="D181" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="E181" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -6485,7 +6485,7 @@
         <v>lang$ui(181)</v>
       </c>
       <c r="D182" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="E182" t="s">
         <v>183</v>
@@ -6503,10 +6503,10 @@
         <v>lang$ui(182)</v>
       </c>
       <c r="D183" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="E183" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -6521,10 +6521,10 @@
         <v>lang$ui(183)</v>
       </c>
       <c r="D184" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="E184" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -6539,10 +6539,10 @@
         <v>lang$ui(184)</v>
       </c>
       <c r="D185" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="E185" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -6557,10 +6557,10 @@
         <v>lang$ui(185)</v>
       </c>
       <c r="D186" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E186" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -6575,10 +6575,10 @@
         <v>lang$ui(186)</v>
       </c>
       <c r="D187" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E187" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -6593,10 +6593,10 @@
         <v>lang$ui(187)</v>
       </c>
       <c r="D188" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="E188" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
@@ -6611,10 +6611,10 @@
         <v>lang$ui(188)</v>
       </c>
       <c r="D189" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="E189" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -6666,10 +6666,10 @@
         <v>lang$server(1)</v>
       </c>
       <c r="D2" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E2" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7953,10 +7953,10 @@
         <v>lang$server(74)</v>
       </c>
       <c r="D75" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E75" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -8667,10 +8667,10 @@
         <v>lang$server(114)</v>
       </c>
       <c r="D115" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E115" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -9009,10 +9009,10 @@
         <v>lang$server(133)</v>
       </c>
       <c r="D134" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="E134" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -9045,10 +9045,10 @@
         <v>lang$server(135)</v>
       </c>
       <c r="D136" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E136" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -9063,10 +9063,10 @@
         <v>lang$server(136)</v>
       </c>
       <c r="D137" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E137" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -9081,10 +9081,10 @@
         <v>lang$server(137)</v>
       </c>
       <c r="D138" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="E138" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -9099,10 +9099,10 @@
         <v>lang$server(138)</v>
       </c>
       <c r="D139" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="E139" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -9117,10 +9117,10 @@
         <v>lang$server(139)</v>
       </c>
       <c r="D140" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="E140" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>